<commit_message>
girdsearch returns now same as default, but dict must be used as scoring parameter
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -425,7 +425,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,7 +445,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
before multiclass selection adaption
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Prio</t>
   </si>
@@ -42,9 +42,6 @@
     <t>variable_importance:. Add code for scikit defautl usage</t>
   </si>
   <si>
-    <t>plot partial dep</t>
-  </si>
-  <si>
     <t>model_comparison: use only df_tune as name</t>
   </si>
   <si>
@@ -63,10 +60,25 @@
     <t>embedding</t>
   </si>
   <si>
-    <t>shap2PD</t>
+    <t>plot partial dep multiclass</t>
+  </si>
+  <si>
+    <t>shap2pd aggregation</t>
   </si>
   <si>
     <t>plot shapley multiclass</t>
+  </si>
+  <si>
+    <t>own spline</t>
+  </si>
+  <si>
+    <t>patialdep plot no multiclass</t>
+  </si>
+  <si>
+    <t>plot my shap (no multiclass)</t>
+  </si>
+  <si>
+    <t>adapt interpret with multiclass selection on "very-high"</t>
   </si>
 </sst>
 </file>
@@ -425,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C293"/>
+  <dimension ref="A1:C292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,43 +485,43 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>8</v>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -518,15 +530,33 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="21" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+    </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
     </row>
@@ -1327,9 +1357,6 @@
     </row>
     <row r="292" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B292" s="3"/>
-    </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B293" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>